<commit_message>
adding profits to tables
</commit_message>
<xml_diff>
--- a/Sep19/all_countries/Tables/groups.xlsx
+++ b/Sep19/all_countries/Tables/groups.xlsx
@@ -14,9 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>M_ETR</t>
+  </si>
+  <si>
+    <t>M_PL</t>
   </si>
   <si>
     <t>GFA - Sales</t>
@@ -431,15 +434,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -468,324 +471,357 @@
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>0.2084179522468874</v>
       </c>
       <c r="C2">
+        <v>139352925129</v>
+      </c>
+      <c r="D2">
         <v>3.495122291891863</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>2.775774459360986</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>2.500693622141029</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>2.017429989315409</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>-0.109960854830155</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>-0.1448485322888229</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>-0.5498042741507762</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>-0.7242426614441151</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>0.2213307288476244</v>
       </c>
       <c r="C3">
+        <v>1017808846331</v>
+      </c>
+      <c r="D3">
         <v>2.499019988544947</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>3.090979343917925</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>2.749696733824161</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>3.147379767852597</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>1.269094571616429</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>1.297804030552637</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>6.345472858082149</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>6.489020152763175</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>0.3720453617170856</v>
       </c>
       <c r="C4">
+        <v>41087099249</v>
+      </c>
+      <c r="D4">
         <v>0.6006099237537484</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>3.428731144937843</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>0.505747365869219</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>2.405701843541175</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.1165861048686212</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0.2537472618454155</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0.5829305243431062</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>1.268736309227077</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <v>0.4804756408017154</v>
       </c>
       <c r="C5">
+        <v>47942268783</v>
+      </c>
+      <c r="D5">
         <v>1.132095450879255</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>5.143782684537935</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>1.105989712654666</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>3.801073312861165</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>0.1684478939786518</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>0.3630108633011897</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>0.8422394698932596</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>1.815054316505949</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>0.2096734066447806</v>
       </c>
       <c r="C6">
+        <v>959424197928</v>
+      </c>
+      <c r="D6">
         <v>3.836192527908431</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>2.314780871820071</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>4.250911976949065</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>3.228815446321175</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>2.25656634707553</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>2.18277934621293</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>11.28283173537765</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>10.91389673106463</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7">
         <v>0.4448419167008774</v>
       </c>
       <c r="C7">
+        <v>38137333219</v>
+      </c>
+      <c r="D7">
         <v>1.631392547285476</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>9.576723308432038</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>2.170876401901705</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>7.508613215709407</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>0.2826686778923709</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>0.6680095719103069</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>1.413343389461855</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>3.340047859551533</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8">
         <v>0.2684919396530561</v>
       </c>
       <c r="C8">
+        <v>91572151625</v>
+      </c>
+      <c r="D8">
         <v>2.544342501865657</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>2.852663773530978</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>2.061815722023631</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>2.268948420676758</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>0.3604700311485228</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>0.3754233160450117</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>1.802350155742614</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>1.877116580225058</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>0.2155134395473036</v>
       </c>
       <c r="C9">
+        <v>1068114426119</v>
+      </c>
+      <c r="D9">
         <v>3.56387865062508</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>2.547287836728417</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>3.733530713081672</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>3.05057686571637</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>1.516147878639397</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>1.466844202700195</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>7.580739393196987</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>7.334221013500969</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B10">
         <v>0.2677170742865432</v>
       </c>
       <c r="C10">
+        <v>200262379816</v>
+      </c>
+      <c r="D10">
         <v>2.716848850876077</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>2.946906456898569</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>2.276159811881235</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>2.430714353394812</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>0.138656677293343</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>0.1498142497400236</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>0.6932833864667144</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>0.7490712487001174</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11">
         <v>0.2034671187804626</v>
       </c>
       <c r="C11">
+        <v>867852046303</v>
+      </c>
+      <c r="D11">
         <v>5.713297586531789</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>1.533217458579776</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>7.431748429398017</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>4.623537134690935</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>5.011663234882424</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>4.808933372275784</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>25.05831617441214</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>24.04466686137889</v>
       </c>
     </row>

</xml_diff>

<commit_message>
stateless entities outside the US
</commit_message>
<xml_diff>
--- a/Sep19/all_countries/Tables/groups.xlsx
+++ b/Sep19/all_countries/Tables/groups.xlsx
@@ -28,16 +28,16 @@
     <t>GFA - Sales + Emp</t>
   </si>
   <si>
+    <t>IMF (20%) - Sales</t>
+  </si>
+  <si>
+    <t>IMF (20%) - Sales + Emp</t>
+  </si>
+  <si>
     <t>IMF - Sales</t>
   </si>
   <si>
     <t>IMF - Sales + Emp</t>
-  </si>
-  <si>
-    <t>OECD (20%) - Sales</t>
-  </si>
-  <si>
-    <t>OECD (20%) - Sales + Emp</t>
   </si>
   <si>
     <t>OECD - Sales</t>
@@ -492,16 +492,16 @@
         <v>2.775774459360986</v>
       </c>
       <c r="F2">
+        <v>0.5001387244282065</v>
+      </c>
+      <c r="G2">
+        <v>0.4034859978630822</v>
+      </c>
+      <c r="H2">
         <v>2.500693622141029</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>2.017429989315409</v>
-      </c>
-      <c r="H2">
-        <v>-0.109960854830155</v>
-      </c>
-      <c r="I2">
-        <v>-0.1448485322888229</v>
       </c>
       <c r="J2">
         <v>-0.5498042741507762</v>
@@ -527,16 +527,16 @@
         <v>3.090979343917925</v>
       </c>
       <c r="F3">
+        <v>0.5499393467648322</v>
+      </c>
+      <c r="G3">
+        <v>0.629475953570518</v>
+      </c>
+      <c r="H3">
         <v>2.749696733824161</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>3.147379767852597</v>
-      </c>
-      <c r="H3">
-        <v>1.269094571616429</v>
-      </c>
-      <c r="I3">
-        <v>1.297804030552637</v>
       </c>
       <c r="J3">
         <v>6.345472858082149</v>
@@ -562,16 +562,16 @@
         <v>3.428731144937843</v>
       </c>
       <c r="F4">
+        <v>0.1011494731738439</v>
+      </c>
+      <c r="G4">
+        <v>0.4811403687082352</v>
+      </c>
+      <c r="H4">
         <v>0.505747365869219</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>2.405701843541175</v>
-      </c>
-      <c r="H4">
-        <v>0.1165861048686212</v>
-      </c>
-      <c r="I4">
-        <v>0.2537472618454155</v>
       </c>
       <c r="J4">
         <v>0.5829305243431062</v>
@@ -597,16 +597,16 @@
         <v>5.143782684537935</v>
       </c>
       <c r="F5">
+        <v>0.2211979425309333</v>
+      </c>
+      <c r="G5">
+        <v>0.7602146625722329</v>
+      </c>
+      <c r="H5">
         <v>1.105989712654666</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>3.801073312861165</v>
-      </c>
-      <c r="H5">
-        <v>0.1684478939786518</v>
-      </c>
-      <c r="I5">
-        <v>0.3630108633011897</v>
       </c>
       <c r="J5">
         <v>0.8422394698932596</v>
@@ -632,16 +632,16 @@
         <v>2.314780871820071</v>
       </c>
       <c r="F6">
+        <v>0.8501823953898133</v>
+      </c>
+      <c r="G6">
+        <v>0.6457630892642331</v>
+      </c>
+      <c r="H6">
         <v>4.250911976949065</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>3.228815446321175</v>
-      </c>
-      <c r="H6">
-        <v>2.25656634707553</v>
-      </c>
-      <c r="I6">
-        <v>2.18277934621293</v>
       </c>
       <c r="J6">
         <v>11.28283173537765</v>
@@ -667,16 +667,16 @@
         <v>9.576723308432038</v>
       </c>
       <c r="F7">
+        <v>0.4341752803803408</v>
+      </c>
+      <c r="G7">
+        <v>1.501722643141881</v>
+      </c>
+      <c r="H7">
         <v>2.170876401901705</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>7.508613215709407</v>
-      </c>
-      <c r="H7">
-        <v>0.2826686778923709</v>
-      </c>
-      <c r="I7">
-        <v>0.6680095719103069</v>
       </c>
       <c r="J7">
         <v>1.413343389461855</v>
@@ -702,16 +702,16 @@
         <v>2.852663773530978</v>
       </c>
       <c r="F8">
+        <v>0.4123631444047267</v>
+      </c>
+      <c r="G8">
+        <v>0.4537896841353516</v>
+      </c>
+      <c r="H8">
         <v>2.061815722023631</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <v>2.268948420676758</v>
-      </c>
-      <c r="H8">
-        <v>0.3604700311485228</v>
-      </c>
-      <c r="I8">
-        <v>0.3754233160450117</v>
       </c>
       <c r="J8">
         <v>1.802350155742614</v>
@@ -737,16 +737,16 @@
         <v>2.547287836728417</v>
       </c>
       <c r="F9">
+        <v>0.7467061426163347</v>
+      </c>
+      <c r="G9">
+        <v>0.6101153731432726</v>
+      </c>
+      <c r="H9">
         <v>3.733530713081672</v>
       </c>
-      <c r="G9">
+      <c r="I9">
         <v>3.05057686571637</v>
-      </c>
-      <c r="H9">
-        <v>1.516147878639397</v>
-      </c>
-      <c r="I9">
-        <v>1.466844202700195</v>
       </c>
       <c r="J9">
         <v>7.580739393196987</v>
@@ -772,16 +772,16 @@
         <v>2.946906456898569</v>
       </c>
       <c r="F10">
+        <v>0.4552319623762475</v>
+      </c>
+      <c r="G10">
+        <v>0.4861428706789624</v>
+      </c>
+      <c r="H10">
         <v>2.276159811881235</v>
       </c>
-      <c r="G10">
+      <c r="I10">
         <v>2.430714353394812</v>
-      </c>
-      <c r="H10">
-        <v>0.138656677293343</v>
-      </c>
-      <c r="I10">
-        <v>0.1498142497400236</v>
       </c>
       <c r="J10">
         <v>0.6932833864667144</v>
@@ -807,16 +807,16 @@
         <v>1.533217458579776</v>
       </c>
       <c r="F11">
+        <v>1.486349685879603</v>
+      </c>
+      <c r="G11">
+        <v>0.9247074269381814</v>
+      </c>
+      <c r="H11">
         <v>7.431748429398017</v>
       </c>
-      <c r="G11">
+      <c r="I11">
         <v>4.623537134690935</v>
-      </c>
-      <c r="H11">
-        <v>5.011663234882424</v>
-      </c>
-      <c r="I11">
-        <v>4.808933372275784</v>
       </c>
       <c r="J11">
         <v>25.05831617441214</v>

</xml_diff>